<commit_message>
update results 2 stat
</commit_message>
<xml_diff>
--- a/Teaching/2018-2019/Stat web page/results/Tabel_Statistica_2018_2019_v3.xlsx
+++ b/Teaching/2018-2019/Stat web page/results/Tabel_Statistica_2018_2019_v3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA47AA41-FC82-4EB1-B05A-9C718EDEDB1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3D7A0-0087-42EE-A8E0-2D0C119F056C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,17 +485,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -513,72 +503,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -927,7 +851,7 @@
   <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
@@ -1016,7 +940,7 @@
       </c>
       <c r="H2">
         <f>Proiect!C2</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I2">
         <f>SUMPRODUCT(Examen!C2:F2,Weights!$B$8:$E$8)</f>
@@ -1495,7 +1419,7 @@
       </c>
       <c r="H11">
         <f>Proiect!C11</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="I11">
         <f>SUMPRODUCT(Examen!C11:F11,Weights!$B$8:$E$8)</f>
@@ -2795,7 +2719,7 @@
       </c>
       <c r="H36">
         <f>Proiect!C36</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I36">
         <f>SUMPRODUCT(Examen!C36:F36,Weights!$B$8:$E$8)</f>
@@ -2803,11 +2727,11 @@
       </c>
       <c r="J36">
         <f xml:space="preserve"> IF(I36&gt;=O$2, MAX(4, ROUND(MIN(10, 1 + 0.6*(C36/(10*SUM(Weights!$B$2:$J$2))+D36/(10*SUM(Weights!$B$3:$G$3))+E36/(10*SUM(Weights!$B$4:$H$4))+F36/(10*SUM(Weights!$B$5:$G$5))+G36/(10*SUM(Weights!$B$6:$G$6))) + I36/30*7 + H36/100),0)), 4)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K36">
         <f xml:space="preserve"> IF(I36&gt;11, MAX(4, ROUND(MIN(10, 1 + 0.6*(C36/(10*SUM(Weights!$B$2:$J$2))+D36/(10*SUM(Weights!$B$3:$G$3))+E36/(10*SUM(Weights!$B$4:$H$4))+F36/(10*SUM(Weights!$B$5:$G$5))+G36/(10*SUM(Weights!$B$6:$G$6))) + I36/30*7 + H36/100),0)), 4)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M36">
         <f>C36/(10*SUM(Weights!$B$2:$J$2))+D36/(10*SUM(Weights!$B$3:$G$3))+E36/(10*SUM(Weights!$B$4:$H$4))+F36/(10*SUM(Weights!$B$5:$G$5))+G36/(10*SUM(Weights!$B$6:$G$6))</f>
@@ -2815,7 +2739,7 @@
       </c>
       <c r="N36">
         <f xml:space="preserve"> MIN(10, 1 + 0.6*(C36/(10*SUM(Weights!$B$2:$J$2))+D36/(10*SUM(Weights!$B$3:$G$3))+E36/(10*SUM(Weights!$B$4:$H$4))+F36/(10*SUM(Weights!$B$5:$G$5))+G36/(10*SUM(Weights!$B$6:$G$6))) + I36/30*7 + H36/100)</f>
-        <v>7.3009523809523813</v>
+        <v>8.8009523809523813</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -4745,37 +4669,37 @@
   </sheetData>
   <autoFilter ref="A1:J73" xr:uid="{59784E6C-1901-43DF-AF93-FE666948192D}"/>
   <conditionalFormatting sqref="I2:I73">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J73">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N73">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>4.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>4.3</formula>
       <formula>4.99</formula>
     </cfRule>
@@ -13731,8 +13655,8 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13759,7 +13683,7 @@
         <v>301</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -13840,7 +13764,7 @@
         <v>301</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -14074,6 +13998,9 @@
       </c>
       <c r="B36">
         <v>311</v>
+      </c>
+      <c r="C36">
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update results stat 2019
</commit_message>
<xml_diff>
--- a/Teaching/2018-2019/Stat web page/results/Tabel_Statistica_2018_2019_v3.xlsx
+++ b/Teaching/2018-2019/Stat web page/results/Tabel_Statistica_2018_2019_v3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3D7A0-0087-42EE-A8E0-2D0C119F056C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{8984D587-EF64-4C13-AD65-F0374DDE78F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{171D9DD5-5907-4E58-AF05-DAFF2CF8E5B9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -851,8 +851,8 @@
   <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M78" sqref="M78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +971,7 @@
       </c>
       <c r="Q2">
         <f xml:space="preserve"> COUNTIF(J2:J73, "= 4") - COUNTIF(I2:I73, "= 0")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="G36">
         <f>SUMPRODUCT(Tema5!C36:H36,Weights!$B$6:$G$6)</f>
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H36">
         <f>Proiect!C36</f>
@@ -2735,11 +2735,11 @@
       </c>
       <c r="M36">
         <f>C36/(10*SUM(Weights!$B$2:$J$2))+D36/(10*SUM(Weights!$B$3:$G$3))+E36/(10*SUM(Weights!$B$4:$H$4))+F36/(10*SUM(Weights!$B$5:$G$5))+G36/(10*SUM(Weights!$B$6:$G$6))</f>
-        <v>4.6682539682539685</v>
+        <v>4.818253968253968</v>
       </c>
       <c r="N36">
         <f xml:space="preserve"> MIN(10, 1 + 0.6*(C36/(10*SUM(Weights!$B$2:$J$2))+D36/(10*SUM(Weights!$B$3:$G$3))+E36/(10*SUM(Weights!$B$4:$H$4))+F36/(10*SUM(Weights!$B$5:$G$5))+G36/(10*SUM(Weights!$B$6:$G$6))) + I36/30*7 + H36/100)</f>
-        <v>8.8009523809523813</v>
+        <v>8.8909523809523812</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -4323,11 +4323,11 @@
       </c>
       <c r="F67">
         <f>SUMPRODUCT(Tema4!C67:H67,Weights!$B$5:$G$5)</f>
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="G67">
         <f>SUMPRODUCT(Tema5!C67:H67,Weights!$B$6:$G$6)</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="H67">
         <f>Proiect!C67</f>
@@ -4339,19 +4339,19 @@
       </c>
       <c r="J67">
         <f xml:space="preserve"> IF(I67&gt;=O$2, MAX(4, ROUND(MIN(10, 1 + 0.6*(C67/(10*SUM(Weights!$B$2:$J$2))+D67/(10*SUM(Weights!$B$3:$G$3))+E67/(10*SUM(Weights!$B$4:$H$4))+F67/(10*SUM(Weights!$B$5:$G$5))+G67/(10*SUM(Weights!$B$6:$G$6))) + I67/30*7 + H67/100),0)), 4)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K67">
         <f xml:space="preserve"> IF(I67&gt;11, MAX(4, ROUND(MIN(10, 1 + 0.6*(C67/(10*SUM(Weights!$B$2:$J$2))+D67/(10*SUM(Weights!$B$3:$G$3))+E67/(10*SUM(Weights!$B$4:$H$4))+F67/(10*SUM(Weights!$B$5:$G$5))+G67/(10*SUM(Weights!$B$6:$G$6))) + I67/30*7 + H67/100),0)), 4)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M67">
         <f>C67/(10*SUM(Weights!$B$2:$J$2))+D67/(10*SUM(Weights!$B$3:$G$3))+E67/(10*SUM(Weights!$B$4:$H$4))+F67/(10*SUM(Weights!$B$5:$G$5))+G67/(10*SUM(Weights!$B$6:$G$6))</f>
-        <v>0</v>
+        <v>1.9166666666666665</v>
       </c>
       <c r="N67">
         <f xml:space="preserve"> MIN(10, 1 + 0.6*(C67/(10*SUM(Weights!$B$2:$J$2))+D67/(10*SUM(Weights!$B$3:$G$3))+E67/(10*SUM(Weights!$B$4:$H$4))+F67/(10*SUM(Weights!$B$5:$G$5))+G67/(10*SUM(Weights!$B$6:$G$6))) + I67/30*7 + H67/100)</f>
-        <v>3.8000000000000003</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -9592,7 +9592,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10911,6 +10911,24 @@
       </c>
       <c r="B67">
         <v>321</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>8</v>
+      </c>
+      <c r="E67">
+        <v>9</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>10</v>
+      </c>
+      <c r="H67">
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -11063,8 +11081,8 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L72" sqref="L72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11442,7 +11460,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -11468,7 +11486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -11494,7 +11512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -11517,7 +11535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -11543,7 +11561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -11569,7 +11587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -11577,7 +11595,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -11603,7 +11621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -11611,7 +11629,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -11637,7 +11655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -11663,7 +11681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -11689,7 +11707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -11697,7 +11715,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -11723,7 +11741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -11749,7 +11767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -11772,7 +11790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -11791,11 +11809,14 @@
       <c r="F36">
         <v>10</v>
       </c>
+      <c r="G36">
+        <v>9</v>
+      </c>
       <c r="H36">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -11803,7 +11824,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -11829,7 +11850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -11855,7 +11876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -11881,7 +11902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -11907,7 +11928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -11933,7 +11954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -11953,7 +11974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -11979,7 +12000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -12005,7 +12026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -12031,7 +12052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -12039,7 +12060,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -12047,7 +12068,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -12070,7 +12091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -12371,6 +12392,24 @@
       </c>
       <c r="B67">
         <v>321</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>10</v>
+      </c>
+      <c r="E67">
+        <v>8</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>10</v>
+      </c>
+      <c r="H67">
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -12500,6 +12539,7 @@
   <autoFilter ref="A1:H73" xr:uid="{6AF7F7A2-6D40-4313-8511-C6424C1AFC85}">
     <filterColumn colId="1">
       <filters>
+        <filter val="311"/>
         <filter val="321"/>
       </filters>
     </filterColumn>
@@ -13655,8 +13695,8 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>